<commit_message>
Fix repository and include new funcionality (generate new hash code after alterations)
</commit_message>
<xml_diff>
--- a/sources/PLANILHA_ALTERA_DESPESA.xlsx
+++ b/sources/PLANILHA_ALTERA_DESPESA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ffmbr-my.sharepoint.com/personal/eliasp_ffm_br/Documents/altera_xml/REFATORAR_ALTERA_XML/sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliasp\Documents\GitHub\python-automatics-data-alterations-in-xml-file\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="264" documentId="8_{FB11FB3F-B50B-4278-9CDC-E7CE1F800870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45E1369D-D87B-436C-9ED8-A84B7A345CC9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE1E47E-9658-48E2-9C5F-9909A7BC3E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2CB27820-A556-4FB3-A9D8-7569D697D985}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{2CB27820-A556-4FB3-A9D8-7569D697D985}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>nr_conta</t>
   </si>
@@ -60,27 +60,6 @@
     <t>new_unidM</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>036</t>
-  </si>
-  <si>
-    <t>040</t>
-  </si>
-  <si>
-    <t>78997500</t>
-  </si>
-  <si>
-    <t>9999999</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
     <t>cod</t>
   </si>
   <si>
@@ -89,24 +68,12 @@
   <si>
     <t>new_vlr</t>
   </si>
-  <si>
-    <t>99999917</t>
-  </si>
-  <si>
-    <t>12,72</t>
-  </si>
-  <si>
-    <t>13,00</t>
-  </si>
-  <si>
-    <t>1556666</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,13 +87,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF535353"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0E0E0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -141,38 +120,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -230,34 +191,30 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{85B1F556-4732-4418-B94B-898810A3A352}" name="Tabela13" displayName="Tabela13" ref="A1:G4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{85B1F556-4732-4418-B94B-898810A3A352}" name="Tabela13" displayName="Tabela13" ref="A1:G4" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:G4" xr:uid="{85B1F556-4732-4418-B94B-898810A3A352}"/>
   <tableColumns count="7">
-    <tableColumn id="13" xr3:uid="{76A2E480-B71B-42BF-8C12-04854B133A08}" name="nr_conta" dataDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{1C128478-DCB8-4EE0-A2EA-0179F6564A25}" name="old_cod" dataDxfId="11" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{192DAD45-D9CC-4B01-867D-AE4BCC975DAB}" name="new_cod" dataDxfId="10" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{892B31F4-BDAF-4D4F-BB11-95B930583EEB}" name="old_tipoT" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{0DC4EA1C-95C4-4E67-8D90-26BAA3E071F8}" name="new_tipoT" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{653771AE-85CB-4906-A207-14B15DE69D6F}" name="old_unidM" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{25FF0592-2163-461B-83C0-A568FE200326}" name="new_unidM" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{76A2E480-B71B-42BF-8C12-04854B133A08}" name="nr_conta" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{1C128478-DCB8-4EE0-A2EA-0179F6564A25}" name="old_cod" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{192DAD45-D9CC-4B01-867D-AE4BCC975DAB}" name="new_cod" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{892B31F4-BDAF-4D4F-BB11-95B930583EEB}" name="old_tipoT" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{0DC4EA1C-95C4-4E67-8D90-26BAA3E071F8}" name="new_tipoT" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{653771AE-85CB-4906-A207-14B15DE69D6F}" name="old_unidM" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{25FF0592-2163-461B-83C0-A568FE200326}" name="new_unidM" dataDxfId="3" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}" name="Tabela3" displayName="Tabela3" ref="A1:D3" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D3" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}" name="Tabela3" displayName="Tabela3" ref="A1:D43" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:D43" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E041450B-B9A8-4984-80F1-F392EA1249E0}" name="nr_conta" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{34DF0F1F-4A50-4495-9A62-004334AB22FA}" name="cod" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{AA7D6B72-0CFC-4D03-95C6-61EB48D14747}" name="old_vlr" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{3D107E8F-238F-4D9E-A978-F4020F61C26E}" name="new_vlr" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E041450B-B9A8-4984-80F1-F392EA1249E0}" name="nr_conta" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{34DF0F1F-4A50-4495-9A62-004334AB22FA}" name="cod"/>
+    <tableColumn id="3" xr3:uid="{AA7D6B72-0CFC-4D03-95C6-61EB48D14747}" name="old_vlr"/>
+    <tableColumn id="4" xr3:uid="{3D107E8F-238F-4D9E-A978-F4020F61C26E}" name="new_vlr"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -562,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C61B51D-8349-4064-B6F9-68B2ADB2D555}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,57 +559,29 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>22105449</v>
-      </c>
-      <c r="B2" s="2">
-        <v>77777721</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2">
-        <v>6</v>
-      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>22106869</v>
-      </c>
-      <c r="B3" s="2">
-        <v>77777721</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2">
-        <v>18</v>
-      </c>
-      <c r="E3" s="2">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
@@ -668,10 +597,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659A0C52-99B9-496E-B347-5D1AC694609B}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,52 +617,518 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>22105449</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1">
-        <v>24.91</v>
-      </c>
-      <c r="D2" s="1">
-        <v>25</v>
+      <c r="A2" s="1"/>
+      <c r="B2" s="3">
+        <v>90056671</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3.93</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
+      <c r="B3" s="3">
+        <v>90206789</v>
+      </c>
+      <c r="C3" s="3">
+        <v>24.41</v>
+      </c>
+      <c r="D3" s="3">
+        <v>22.07</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="3">
+        <v>90330048</v>
+      </c>
+      <c r="C4" s="3">
+        <v>18.09</v>
+      </c>
+      <c r="D4" s="3">
+        <v>16.36</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="3">
+        <v>90395972</v>
+      </c>
+      <c r="C5" s="3">
+        <v>9.16</v>
+      </c>
+      <c r="D5" s="3">
+        <v>8.7899999999999991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3">
+        <v>90408756</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.64</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3">
+        <v>90294220</v>
+      </c>
+      <c r="C7" s="3">
+        <v>101.56</v>
+      </c>
+      <c r="D7" s="3">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3">
+        <v>90096924</v>
+      </c>
+      <c r="C8" s="3">
+        <v>17.8</v>
+      </c>
+      <c r="D8" s="3">
+        <v>17.09</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3">
+        <v>90466314</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2.17</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3">
+        <v>90058666</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3">
+        <v>90222377</v>
+      </c>
+      <c r="C11" s="3">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="D11" s="3">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3">
+        <v>90310500</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.21</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3">
+        <v>90521811</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3">
+        <v>90159535</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.27</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3">
+        <v>90086252</v>
+      </c>
+      <c r="C15" s="3">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3">
+        <v>90056671</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3">
+        <v>90206789</v>
+      </c>
+      <c r="C17" s="3">
+        <v>24.41</v>
+      </c>
+      <c r="D17" s="3">
+        <v>22.07</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="3">
+        <v>90330048</v>
+      </c>
+      <c r="C18" s="3">
+        <v>18.09</v>
+      </c>
+      <c r="D18" s="3">
+        <v>16.36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3">
+        <v>90395972</v>
+      </c>
+      <c r="C19" s="3">
+        <v>9.16</v>
+      </c>
+      <c r="D19" s="3">
+        <v>8.7899999999999991</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="3">
+        <v>90408756</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1.64</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="3">
+        <v>90294220</v>
+      </c>
+      <c r="C21" s="3">
+        <v>101.56</v>
+      </c>
+      <c r="D21" s="3">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="3">
+        <v>90096924</v>
+      </c>
+      <c r="C22" s="3">
+        <v>17.8</v>
+      </c>
+      <c r="D22" s="3">
+        <v>17.09</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="3">
+        <v>90466314</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2.17</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="3">
+        <v>90058666</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="3">
+        <v>90222377</v>
+      </c>
+      <c r="C25" s="3">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="D25" s="3">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="3">
+        <v>90310500</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1.21</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="3">
+        <v>90521811</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="3">
+        <v>90159535</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1.27</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="3">
+        <v>90086252</v>
+      </c>
+      <c r="C29" s="3">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="D29" s="3">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="3">
+        <v>90056671</v>
+      </c>
+      <c r="C30" s="3">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="D30" s="3">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="3">
+        <v>90206789</v>
+      </c>
+      <c r="C31" s="3">
+        <v>24.41</v>
+      </c>
+      <c r="D31" s="3">
+        <v>22.07</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="3">
+        <v>90330048</v>
+      </c>
+      <c r="C32" s="3">
+        <v>18.09</v>
+      </c>
+      <c r="D32" s="3">
+        <v>16.36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="3">
+        <v>90395972</v>
+      </c>
+      <c r="C33" s="3">
+        <v>9.16</v>
+      </c>
+      <c r="D33" s="3">
+        <v>8.7899999999999991</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="3">
+        <v>90408756</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1.64</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="3">
+        <v>90294220</v>
+      </c>
+      <c r="C35" s="3">
+        <v>101.56</v>
+      </c>
+      <c r="D35" s="3">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="3">
+        <v>90096924</v>
+      </c>
+      <c r="C36" s="3">
+        <v>17.8</v>
+      </c>
+      <c r="D36" s="3">
+        <v>17.09</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="3">
+        <v>90466314</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2.17</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="3">
+        <v>90058666</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="3">
+        <v>90222377</v>
+      </c>
+      <c r="C39" s="3">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="D39" s="3">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="3">
+        <v>90310500</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1.21</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="3">
+        <v>90521811</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="3">
+        <v>90159535</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1.27</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="3">
+        <v>90086252</v>
+      </c>
+      <c r="C43" s="3">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="D43" s="3">
+        <v>3.68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>